<commit_message>
updated modules 7 and 8 and lab 7-1
</commit_message>
<xml_diff>
--- a/modules/lab7/CEE348_dye_data_Lab7.xlsx
+++ b/modules/lab7/CEE348_dye_data_Lab7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdlund/Documents/CEE348_EnvE_Environmental_flows_class/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F146E61-E1AF-844E-B955-726FD139D886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E936A5-8F29-E14A-81D3-E09762F74400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="725" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4720" yWindow="460" windowWidth="28800" windowHeight="15960" tabRatio="725" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GA050630a" sheetId="20" r:id="rId1"/>
@@ -380,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -466,6 +466,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6690,7 +6691,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="10300" topLeftCell="A203"/>
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="E49" sqref="E49:E66"/>
     </sheetView>
   </sheetViews>
@@ -6770,8 +6771,8 @@
         <v>14</v>
       </c>
       <c r="B4" s="13">
-        <f>B3*0.02832</f>
-        <v>385.58875494013199</v>
+        <f>B3*0.0353147</f>
+        <v>480.82454816681775</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>13</v>
@@ -12649,7 +12650,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="10300" topLeftCell="A203"/>
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="E49" sqref="E49:E66"/>
     </sheetView>
   </sheetViews>
@@ -12729,8 +12730,8 @@
         <v>14</v>
       </c>
       <c r="B4" s="13">
-        <f>B3*0.02832</f>
-        <v>1818.9381552436296</v>
+        <f>B3*0.0353147</f>
+        <v>2268.1940420544561</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>13</v>
@@ -18510,9 +18511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10300" topLeftCell="A203"/>
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="E49" sqref="E49:E66"/>
     </sheetView>
   </sheetViews>
@@ -18592,8 +18593,8 @@
         <v>14</v>
       </c>
       <c r="B4" s="13">
-        <f>B3*0.02832</f>
-        <v>1748.9693673650745</v>
+        <f>B3*0.0353147</f>
+        <v>2180.9438035906564</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>13</v>
@@ -24209,9 +24210,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O213"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10300" topLeftCell="A203"/>
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="E49" sqref="E49:E66"/>
     </sheetView>
   </sheetViews>
@@ -24291,8 +24292,8 @@
         <v>14</v>
       </c>
       <c r="B4" s="13">
-        <f>B3*0.02832</f>
-        <v>887.70089619573446</v>
+        <f>B3*0.0353147</f>
+        <v>1106.9523601300671</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>13</v>
@@ -30260,7 +30261,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="10300" topLeftCell="A203"/>
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="E49" sqref="E49:E66"/>
     </sheetView>
   </sheetViews>
@@ -30339,8 +30340,8 @@
       <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="13" t="e">
-        <f>B3*0.02832</f>
+      <c r="B4" s="41" t="e">
+        <f>B3*0.0353147</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C4" s="11" t="s">

</xml_diff>